<commit_message>
Add more literature tokens
</commit_message>
<xml_diff>
--- a/pythonProject/evaluation/classla/literature.xlsx
+++ b/pythonProject/evaluation/classla/literature.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="123">
   <si>
     <t>Tag</t>
   </si>
@@ -324,6 +324,45 @@
   </si>
   <si>
     <t>Osećala</t>
+  </si>
+  <si>
+    <t>Jednako</t>
+  </si>
+  <si>
+    <t>Brzim</t>
+  </si>
+  <si>
+    <t>pogledom</t>
+  </si>
+  <si>
+    <t>Bože</t>
+  </si>
+  <si>
+    <t>ime</t>
+  </si>
+  <si>
+    <t>božje</t>
+  </si>
+  <si>
+    <t>Seti</t>
+  </si>
+  <si>
+    <t>Lice</t>
+  </si>
+  <si>
+    <t>Kriv</t>
+  </si>
+  <si>
+    <t>Ti</t>
+  </si>
+  <si>
+    <t>Recite</t>
+  </si>
+  <si>
+    <t>Zar</t>
+  </si>
+  <si>
+    <t>Vaše</t>
   </si>
   <si>
     <t>O</t>
@@ -739,7 +778,7 @@
         <v>0.21</v>
       </c>
       <c r="D2">
-        <v>0.34</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -750,10 +789,10 @@
         <v>0.25</v>
       </c>
       <c r="C3">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="D3">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -761,7 +800,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.82</v>
+        <v>0.84</v>
       </c>
       <c r="C4">
         <v>0.53</v>
@@ -806,10 +845,10 @@
         <v>0.98</v>
       </c>
       <c r="C7">
-        <v>0.86</v>
+        <v>0.8</v>
       </c>
       <c r="D7">
-        <v>0.92</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -820,10 +859,10 @@
         <v>0.65</v>
       </c>
       <c r="C8">
-        <v>0.28</v>
+        <v>0.27</v>
       </c>
       <c r="D8">
-        <v>0.34</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -831,13 +870,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>0.53</v>
+        <v>0.51</v>
       </c>
       <c r="C9">
-        <v>0.84</v>
+        <v>0.85</v>
       </c>
       <c r="D9">
-        <v>0.65</v>
+        <v>0.64</v>
       </c>
     </row>
   </sheetData>
@@ -847,7 +886,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:D133"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -875,7 +914,7 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -889,7 +928,7 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -903,7 +942,7 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
@@ -917,7 +956,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -931,7 +970,7 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -945,7 +984,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -959,7 +998,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
@@ -973,7 +1012,7 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
@@ -987,7 +1026,7 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -1029,7 +1068,7 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
@@ -1043,7 +1082,7 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
@@ -1057,7 +1096,7 @@
         <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
@@ -1071,7 +1110,7 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D16" t="s">
         <v>4</v>
@@ -1085,7 +1124,7 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
@@ -1099,7 +1138,7 @@
         <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
@@ -1113,7 +1152,7 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
@@ -1127,7 +1166,7 @@
         <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
@@ -1141,7 +1180,7 @@
         <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
@@ -1155,7 +1194,7 @@
         <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
@@ -1169,7 +1208,7 @@
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -1183,7 +1222,7 @@
         <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -1197,7 +1236,7 @@
         <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
@@ -1211,7 +1250,7 @@
         <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -1225,7 +1264,7 @@
         <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D27" t="s">
         <v>4</v>
@@ -1239,7 +1278,7 @@
         <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
@@ -1253,7 +1292,7 @@
         <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
@@ -1281,7 +1320,7 @@
         <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
@@ -1295,7 +1334,7 @@
         <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D32" t="s">
         <v>6</v>
@@ -1309,7 +1348,7 @@
         <v>42</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>
@@ -1323,7 +1362,7 @@
         <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D34" t="s">
         <v>8</v>
@@ -1351,7 +1390,7 @@
         <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D36" t="s">
         <v>4</v>
@@ -1379,7 +1418,7 @@
         <v>47</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D38" t="s">
         <v>4</v>
@@ -1393,7 +1432,7 @@
         <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D39" t="s">
         <v>6</v>
@@ -1407,7 +1446,7 @@
         <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D40" t="s">
         <v>6</v>
@@ -1421,7 +1460,7 @@
         <v>50</v>
       </c>
       <c r="C41" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D41" t="s">
         <v>9</v>
@@ -1435,7 +1474,7 @@
         <v>51</v>
       </c>
       <c r="C42" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D42" t="s">
         <v>6</v>
@@ -1463,7 +1502,7 @@
         <v>51</v>
       </c>
       <c r="C44" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
@@ -1477,7 +1516,7 @@
         <v>53</v>
       </c>
       <c r="C45" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
@@ -1505,7 +1544,7 @@
         <v>28</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D47" t="s">
         <v>5</v>
@@ -1519,7 +1558,7 @@
         <v>55</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D48" t="s">
         <v>6</v>
@@ -1533,7 +1572,7 @@
         <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D49" t="s">
         <v>6</v>
@@ -1547,7 +1586,7 @@
         <v>56</v>
       </c>
       <c r="C50" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D50" t="s">
         <v>6</v>
@@ -1561,7 +1600,7 @@
         <v>57</v>
       </c>
       <c r="C51" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D51" t="s">
         <v>6</v>
@@ -1603,7 +1642,7 @@
         <v>60</v>
       </c>
       <c r="C54" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D54" t="s">
         <v>6</v>
@@ -1631,7 +1670,7 @@
         <v>62</v>
       </c>
       <c r="C56" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D56" t="s">
         <v>6</v>
@@ -1645,7 +1684,7 @@
         <v>52</v>
       </c>
       <c r="C57" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D57" t="s">
         <v>6</v>
@@ -1659,7 +1698,7 @@
         <v>63</v>
       </c>
       <c r="C58" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D58" t="s">
         <v>5</v>
@@ -1673,7 +1712,7 @@
         <v>64</v>
       </c>
       <c r="C59" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D59" t="s">
         <v>5</v>
@@ -1687,7 +1726,7 @@
         <v>65</v>
       </c>
       <c r="C60" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D60" t="s">
         <v>6</v>
@@ -1701,7 +1740,7 @@
         <v>66</v>
       </c>
       <c r="C61" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D61" t="s">
         <v>6</v>
@@ -1715,7 +1754,7 @@
         <v>67</v>
       </c>
       <c r="C62" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D62" t="s">
         <v>6</v>
@@ -1729,7 +1768,7 @@
         <v>33</v>
       </c>
       <c r="C63" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D63" t="s">
         <v>6</v>
@@ -1743,7 +1782,7 @@
         <v>33</v>
       </c>
       <c r="C64" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D64" t="s">
         <v>6</v>
@@ -1757,7 +1796,7 @@
         <v>68</v>
       </c>
       <c r="C65" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D65" t="s">
         <v>4</v>
@@ -1771,7 +1810,7 @@
         <v>66</v>
       </c>
       <c r="C66" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D66" t="s">
         <v>5</v>
@@ -1785,7 +1824,7 @@
         <v>39</v>
       </c>
       <c r="C67" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D67" t="s">
         <v>6</v>
@@ -1799,7 +1838,7 @@
         <v>69</v>
       </c>
       <c r="C68" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D68" t="s">
         <v>6</v>
@@ -1827,7 +1866,7 @@
         <v>71</v>
       </c>
       <c r="C70" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D70" t="s">
         <v>6</v>
@@ -1841,7 +1880,7 @@
         <v>72</v>
       </c>
       <c r="C71" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D71" t="s">
         <v>6</v>
@@ -1855,7 +1894,7 @@
         <v>73</v>
       </c>
       <c r="C72" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D72" t="s">
         <v>6</v>
@@ -1869,7 +1908,7 @@
         <v>74</v>
       </c>
       <c r="C73" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D73" t="s">
         <v>6</v>
@@ -1883,7 +1922,7 @@
         <v>75</v>
       </c>
       <c r="C74" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D74" t="s">
         <v>6</v>
@@ -1900,7 +1939,7 @@
         <v>5</v>
       </c>
       <c r="D75" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1914,7 +1953,7 @@
         <v>8</v>
       </c>
       <c r="D76" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1928,7 +1967,7 @@
         <v>8</v>
       </c>
       <c r="D77" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1942,7 +1981,7 @@
         <v>5</v>
       </c>
       <c r="D78" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1956,7 +1995,7 @@
         <v>8</v>
       </c>
       <c r="D79" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1967,7 +2006,7 @@
         <v>78</v>
       </c>
       <c r="C80" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D80" t="s">
         <v>6</v>
@@ -1984,7 +2023,7 @@
         <v>5</v>
       </c>
       <c r="D81" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2023,7 +2062,7 @@
         <v>39</v>
       </c>
       <c r="C84" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D84" t="s">
         <v>6</v>
@@ -2037,7 +2076,7 @@
         <v>82</v>
       </c>
       <c r="C85" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D85" t="s">
         <v>6</v>
@@ -2065,7 +2104,7 @@
         <v>41</v>
       </c>
       <c r="C87" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D87" t="s">
         <v>6</v>
@@ -2079,7 +2118,7 @@
         <v>84</v>
       </c>
       <c r="C88" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D88" t="s">
         <v>4</v>
@@ -2096,7 +2135,7 @@
         <v>6</v>
       </c>
       <c r="D89" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2107,7 +2146,7 @@
         <v>86</v>
       </c>
       <c r="C90" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D90" t="s">
         <v>4</v>
@@ -2121,7 +2160,7 @@
         <v>87</v>
       </c>
       <c r="C91" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D91" t="s">
         <v>5</v>
@@ -2135,7 +2174,7 @@
         <v>61</v>
       </c>
       <c r="C92" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D92" t="s">
         <v>9</v>
@@ -2149,7 +2188,7 @@
         <v>19</v>
       </c>
       <c r="C93" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D93" t="s">
         <v>6</v>
@@ -2163,7 +2202,7 @@
         <v>88</v>
       </c>
       <c r="C94" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D94" t="s">
         <v>6</v>
@@ -2177,7 +2216,7 @@
         <v>89</v>
       </c>
       <c r="C95" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D95" t="s">
         <v>6</v>
@@ -2191,7 +2230,7 @@
         <v>90</v>
       </c>
       <c r="C96" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D96" t="s">
         <v>6</v>
@@ -2205,7 +2244,7 @@
         <v>91</v>
       </c>
       <c r="C97" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D97" t="s">
         <v>6</v>
@@ -2219,7 +2258,7 @@
         <v>92</v>
       </c>
       <c r="C98" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D98" t="s">
         <v>6</v>
@@ -2233,7 +2272,7 @@
         <v>88</v>
       </c>
       <c r="C99" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D99" t="s">
         <v>6</v>
@@ -2247,7 +2286,7 @@
         <v>30</v>
       </c>
       <c r="C100" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D100" t="s">
         <v>6</v>
@@ -2261,7 +2300,7 @@
         <v>93</v>
       </c>
       <c r="C101" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D101" t="s">
         <v>5</v>
@@ -2289,7 +2328,7 @@
         <v>28</v>
       </c>
       <c r="C103" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D103" t="s">
         <v>5</v>
@@ -2303,7 +2342,7 @@
         <v>95</v>
       </c>
       <c r="C104" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D104" t="s">
         <v>4</v>
@@ -2317,7 +2356,7 @@
         <v>96</v>
       </c>
       <c r="C105" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D105" t="s">
         <v>6</v>
@@ -2331,7 +2370,7 @@
         <v>97</v>
       </c>
       <c r="C106" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D106" t="s">
         <v>9</v>
@@ -2345,7 +2384,7 @@
         <v>98</v>
       </c>
       <c r="C107" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D107" t="s">
         <v>6</v>
@@ -2359,7 +2398,7 @@
         <v>74</v>
       </c>
       <c r="C108" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D108" t="s">
         <v>6</v>
@@ -2373,7 +2412,7 @@
         <v>30</v>
       </c>
       <c r="C109" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D109" t="s">
         <v>5</v>
@@ -2387,7 +2426,7 @@
         <v>99</v>
       </c>
       <c r="C110" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D110" t="s">
         <v>6</v>
@@ -2401,7 +2440,7 @@
         <v>74</v>
       </c>
       <c r="C111" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D111" t="s">
         <v>6</v>
@@ -2415,10 +2454,304 @@
         <v>100</v>
       </c>
       <c r="C112" t="s">
+        <v>114</v>
+      </c>
+      <c r="D112" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" t="s">
         <v>101</v>
       </c>
-      <c r="D112" t="s">
-        <v>6</v>
+      <c r="B113" t="s">
+        <v>101</v>
+      </c>
+      <c r="C113" t="s">
+        <v>114</v>
+      </c>
+      <c r="D113" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" t="s">
+        <v>23</v>
+      </c>
+      <c r="B114" t="s">
+        <v>23</v>
+      </c>
+      <c r="C114" t="s">
+        <v>114</v>
+      </c>
+      <c r="D114" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" t="s">
+        <v>102</v>
+      </c>
+      <c r="B115" t="s">
+        <v>102</v>
+      </c>
+      <c r="C115" t="s">
+        <v>114</v>
+      </c>
+      <c r="D115" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" t="s">
+        <v>103</v>
+      </c>
+      <c r="B116" t="s">
+        <v>103</v>
+      </c>
+      <c r="C116" t="s">
+        <v>114</v>
+      </c>
+      <c r="D116" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" t="s">
+        <v>23</v>
+      </c>
+      <c r="B117" t="s">
+        <v>23</v>
+      </c>
+      <c r="C117" t="s">
+        <v>114</v>
+      </c>
+      <c r="D117" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" t="s">
+        <v>67</v>
+      </c>
+      <c r="B118" t="s">
+        <v>67</v>
+      </c>
+      <c r="C118" t="s">
+        <v>114</v>
+      </c>
+      <c r="D118" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" t="s">
+        <v>104</v>
+      </c>
+      <c r="B119" t="s">
+        <v>104</v>
+      </c>
+      <c r="C119" t="s">
+        <v>114</v>
+      </c>
+      <c r="D119" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" t="s">
+        <v>23</v>
+      </c>
+      <c r="B120" t="s">
+        <v>23</v>
+      </c>
+      <c r="C120" t="s">
+        <v>114</v>
+      </c>
+      <c r="D120" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" t="s">
+        <v>93</v>
+      </c>
+      <c r="B121" t="s">
+        <v>93</v>
+      </c>
+      <c r="C121" t="s">
+        <v>114</v>
+      </c>
+      <c r="D121" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" t="s">
+        <v>105</v>
+      </c>
+      <c r="B122" t="s">
+        <v>105</v>
+      </c>
+      <c r="C122" t="s">
+        <v>114</v>
+      </c>
+      <c r="D122" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" t="s">
+        <v>106</v>
+      </c>
+      <c r="B123" t="s">
+        <v>106</v>
+      </c>
+      <c r="C123" t="s">
+        <v>114</v>
+      </c>
+      <c r="D123" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" t="s">
+        <v>107</v>
+      </c>
+      <c r="B124" t="s">
+        <v>107</v>
+      </c>
+      <c r="C124" t="s">
+        <v>114</v>
+      </c>
+      <c r="D124" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" t="s">
+        <v>108</v>
+      </c>
+      <c r="B125" t="s">
+        <v>108</v>
+      </c>
+      <c r="C125" t="s">
+        <v>114</v>
+      </c>
+      <c r="D125" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" t="s">
+        <v>23</v>
+      </c>
+      <c r="B126" t="s">
+        <v>23</v>
+      </c>
+      <c r="C126" t="s">
+        <v>114</v>
+      </c>
+      <c r="D126" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" t="s">
+        <v>67</v>
+      </c>
+      <c r="B127" t="s">
+        <v>67</v>
+      </c>
+      <c r="C127" t="s">
+        <v>114</v>
+      </c>
+      <c r="D127" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" t="s">
+        <v>109</v>
+      </c>
+      <c r="B128" t="s">
+        <v>109</v>
+      </c>
+      <c r="C128" t="s">
+        <v>114</v>
+      </c>
+      <c r="D128" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" t="s">
+        <v>110</v>
+      </c>
+      <c r="B129" t="s">
+        <v>110</v>
+      </c>
+      <c r="C129" t="s">
+        <v>114</v>
+      </c>
+      <c r="D129" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" t="s">
+        <v>111</v>
+      </c>
+      <c r="B130" t="s">
+        <v>111</v>
+      </c>
+      <c r="C130" t="s">
+        <v>114</v>
+      </c>
+      <c r="D130" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" t="s">
+        <v>112</v>
+      </c>
+      <c r="B131" t="s">
+        <v>112</v>
+      </c>
+      <c r="C131" t="s">
+        <v>114</v>
+      </c>
+      <c r="D131" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" t="s">
+        <v>111</v>
+      </c>
+      <c r="B132" t="s">
+        <v>111</v>
+      </c>
+      <c r="C132" t="s">
+        <v>114</v>
+      </c>
+      <c r="D132" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" t="s">
+        <v>113</v>
+      </c>
+      <c r="B133" t="s">
+        <v>113</v>
+      </c>
+      <c r="C133" t="s">
+        <v>114</v>
+      </c>
+      <c r="D133" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2450,44 +2783,44 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="B2">
         <v>0.86</v>
       </c>
       <c r="C2">
-        <v>0.21</v>
+        <v>0.19</v>
       </c>
       <c r="D2">
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="B3">
         <v>0.14</v>
       </c>
       <c r="C3">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="D3">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="B4">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
       <c r="C4">
-        <v>0.65</v>
+        <v>0.62</v>
       </c>
       <c r="D4">
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2495,13 +2828,13 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.63</v>
+        <v>0.64</v>
       </c>
       <c r="C5">
-        <v>0.3</v>
+        <v>0.29</v>
       </c>
       <c r="D5">
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2509,13 +2842,13 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>0.54</v>
+        <v>0.52</v>
       </c>
       <c r="C6">
-        <v>0.86</v>
+        <v>0.87</v>
       </c>
       <c r="D6">
-        <v>0.66</v>
+        <v>0.65</v>
       </c>
     </row>
   </sheetData>
@@ -2525,7 +2858,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:D130"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2553,10 +2886,10 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2567,10 +2900,10 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2581,10 +2914,10 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2595,10 +2928,10 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D5" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2609,10 +2942,10 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2623,10 +2956,10 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D7" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2637,10 +2970,10 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2651,10 +2984,10 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D9" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2665,10 +2998,10 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D10" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2679,10 +3012,10 @@
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="D11" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2693,10 +3026,10 @@
         <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D12" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2707,10 +3040,10 @@
         <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D13" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2721,10 +3054,10 @@
         <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D14" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2735,10 +3068,10 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D15" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2749,10 +3082,10 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D16" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2763,10 +3096,10 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2777,10 +3110,10 @@
         <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D18" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2791,10 +3124,10 @@
         <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D19" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2805,10 +3138,10 @@
         <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D20" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2819,10 +3152,10 @@
         <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D21" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2833,10 +3166,10 @@
         <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D22" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2847,10 +3180,10 @@
         <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D23" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2861,10 +3194,10 @@
         <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D24" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2875,10 +3208,10 @@
         <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D25" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2889,10 +3222,10 @@
         <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2903,10 +3236,10 @@
         <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D27" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2917,10 +3250,10 @@
         <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D28" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2931,10 +3264,10 @@
         <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D29" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2945,10 +3278,10 @@
         <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D30" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2959,10 +3292,10 @@
         <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D31" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2973,10 +3306,10 @@
         <v>42</v>
       </c>
       <c r="C32" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D32" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2987,10 +3320,10 @@
         <v>43</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D33" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -3001,10 +3334,10 @@
         <v>44</v>
       </c>
       <c r="C34" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D34" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -3015,10 +3348,10 @@
         <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -3029,10 +3362,10 @@
         <v>46</v>
       </c>
       <c r="C36" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D36" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -3043,10 +3376,10 @@
         <v>47</v>
       </c>
       <c r="C37" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D37" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -3057,10 +3390,10 @@
         <v>48</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D38" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -3071,10 +3404,10 @@
         <v>49</v>
       </c>
       <c r="C39" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D39" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -3085,10 +3418,10 @@
         <v>50</v>
       </c>
       <c r="C40" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D40" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -3099,10 +3432,10 @@
         <v>51</v>
       </c>
       <c r="C41" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D41" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -3113,10 +3446,10 @@
         <v>52</v>
       </c>
       <c r="C42" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D42" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -3127,10 +3460,10 @@
         <v>51</v>
       </c>
       <c r="C43" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D43" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -3141,10 +3474,10 @@
         <v>53</v>
       </c>
       <c r="C44" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D44" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3155,10 +3488,10 @@
         <v>28</v>
       </c>
       <c r="C45" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D45" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -3169,10 +3502,10 @@
         <v>55</v>
       </c>
       <c r="C46" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D46" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -3183,10 +3516,10 @@
         <v>52</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D47" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -3197,10 +3530,10 @@
         <v>56</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D48" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -3211,10 +3544,10 @@
         <v>57</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D49" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -3225,10 +3558,10 @@
         <v>58</v>
       </c>
       <c r="C50" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D50" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -3239,10 +3572,10 @@
         <v>59</v>
       </c>
       <c r="C51" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D51" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -3253,10 +3586,10 @@
         <v>60</v>
       </c>
       <c r="C52" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D52" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -3267,10 +3600,10 @@
         <v>62</v>
       </c>
       <c r="C53" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D53" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -3281,10 +3614,10 @@
         <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D54" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -3295,10 +3628,10 @@
         <v>63</v>
       </c>
       <c r="C55" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D55" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -3309,10 +3642,10 @@
         <v>64</v>
       </c>
       <c r="C56" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D56" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -3323,10 +3656,10 @@
         <v>65</v>
       </c>
       <c r="C57" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D57" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -3337,10 +3670,10 @@
         <v>66</v>
       </c>
       <c r="C58" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D58" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -3351,10 +3684,10 @@
         <v>67</v>
       </c>
       <c r="C59" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D59" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -3365,10 +3698,10 @@
         <v>33</v>
       </c>
       <c r="C60" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D60" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -3379,10 +3712,10 @@
         <v>33</v>
       </c>
       <c r="C61" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D61" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -3393,10 +3726,10 @@
         <v>68</v>
       </c>
       <c r="C62" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D62" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -3407,10 +3740,10 @@
         <v>66</v>
       </c>
       <c r="C63" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D63" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -3421,10 +3754,10 @@
         <v>39</v>
       </c>
       <c r="C64" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D64" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -3435,10 +3768,10 @@
         <v>69</v>
       </c>
       <c r="C65" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D65" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -3449,10 +3782,10 @@
         <v>70</v>
       </c>
       <c r="C66" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D66" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -3463,10 +3796,10 @@
         <v>71</v>
       </c>
       <c r="C67" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D67" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -3477,10 +3810,10 @@
         <v>72</v>
       </c>
       <c r="C68" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D68" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -3491,10 +3824,10 @@
         <v>73</v>
       </c>
       <c r="C69" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D69" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -3505,10 +3838,10 @@
         <v>74</v>
       </c>
       <c r="C70" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D70" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -3519,10 +3852,10 @@
         <v>75</v>
       </c>
       <c r="C71" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D71" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -3533,10 +3866,10 @@
         <v>76</v>
       </c>
       <c r="C72" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D72" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -3547,10 +3880,10 @@
         <v>77</v>
       </c>
       <c r="C73" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D73" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -3561,10 +3894,10 @@
         <v>77</v>
       </c>
       <c r="C74" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D74" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -3575,10 +3908,10 @@
         <v>76</v>
       </c>
       <c r="C75" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D75" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -3589,10 +3922,10 @@
         <v>77</v>
       </c>
       <c r="C76" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D76" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -3603,10 +3936,10 @@
         <v>78</v>
       </c>
       <c r="C77" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D77" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -3617,10 +3950,10 @@
         <v>79</v>
       </c>
       <c r="C78" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D78" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -3631,10 +3964,10 @@
         <v>80</v>
       </c>
       <c r="C79" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D79" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -3645,10 +3978,10 @@
         <v>81</v>
       </c>
       <c r="C80" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D80" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -3659,10 +3992,10 @@
         <v>39</v>
       </c>
       <c r="C81" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D81" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -3673,10 +4006,10 @@
         <v>82</v>
       </c>
       <c r="C82" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D82" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -3687,10 +4020,10 @@
         <v>83</v>
       </c>
       <c r="C83" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D83" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -3701,10 +4034,10 @@
         <v>41</v>
       </c>
       <c r="C84" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D84" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -3715,10 +4048,10 @@
         <v>84</v>
       </c>
       <c r="C85" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D85" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -3729,10 +4062,10 @@
         <v>85</v>
       </c>
       <c r="C86" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D86" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -3743,10 +4076,10 @@
         <v>86</v>
       </c>
       <c r="C87" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D87" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -3757,10 +4090,10 @@
         <v>87</v>
       </c>
       <c r="C88" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D88" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -3771,10 +4104,10 @@
         <v>61</v>
       </c>
       <c r="C89" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D89" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -3785,10 +4118,10 @@
         <v>19</v>
       </c>
       <c r="C90" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D90" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -3799,10 +4132,10 @@
         <v>88</v>
       </c>
       <c r="C91" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D91" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -3813,10 +4146,10 @@
         <v>89</v>
       </c>
       <c r="C92" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D92" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -3827,10 +4160,10 @@
         <v>90</v>
       </c>
       <c r="C93" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D93" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -3841,10 +4174,10 @@
         <v>91</v>
       </c>
       <c r="C94" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D94" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -3855,10 +4188,10 @@
         <v>92</v>
       </c>
       <c r="C95" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D95" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -3869,10 +4202,10 @@
         <v>88</v>
       </c>
       <c r="C96" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D96" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -3883,10 +4216,10 @@
         <v>30</v>
       </c>
       <c r="C97" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D97" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -3897,10 +4230,10 @@
         <v>93</v>
       </c>
       <c r="C98" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D98" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -3911,10 +4244,10 @@
         <v>94</v>
       </c>
       <c r="C99" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D99" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -3925,10 +4258,10 @@
         <v>28</v>
       </c>
       <c r="C100" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D100" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -3939,10 +4272,10 @@
         <v>95</v>
       </c>
       <c r="C101" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D101" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -3953,10 +4286,10 @@
         <v>96</v>
       </c>
       <c r="C102" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D102" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -3967,10 +4300,10 @@
         <v>97</v>
       </c>
       <c r="C103" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D103" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -3981,10 +4314,10 @@
         <v>98</v>
       </c>
       <c r="C104" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D104" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -3995,10 +4328,10 @@
         <v>74</v>
       </c>
       <c r="C105" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D105" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -4009,10 +4342,10 @@
         <v>30</v>
       </c>
       <c r="C106" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D106" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -4023,10 +4356,10 @@
         <v>99</v>
       </c>
       <c r="C107" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D107" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -4037,10 +4370,10 @@
         <v>74</v>
       </c>
       <c r="C108" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D108" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -4051,10 +4384,304 @@
         <v>100</v>
       </c>
       <c r="C109" t="s">
+        <v>114</v>
+      </c>
+      <c r="D109" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" t="s">
         <v>101</v>
       </c>
-      <c r="D109" t="s">
+      <c r="B110" t="s">
+        <v>101</v>
+      </c>
+      <c r="C110" t="s">
+        <v>114</v>
+      </c>
+      <c r="D110" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" t="s">
+        <v>23</v>
+      </c>
+      <c r="B111" t="s">
+        <v>23</v>
+      </c>
+      <c r="C111" t="s">
+        <v>114</v>
+      </c>
+      <c r="D111" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" t="s">
+        <v>102</v>
+      </c>
+      <c r="B112" t="s">
+        <v>102</v>
+      </c>
+      <c r="C112" t="s">
+        <v>114</v>
+      </c>
+      <c r="D112" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" t="s">
+        <v>103</v>
+      </c>
+      <c r="B113" t="s">
+        <v>103</v>
+      </c>
+      <c r="C113" t="s">
+        <v>114</v>
+      </c>
+      <c r="D113" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" t="s">
+        <v>23</v>
+      </c>
+      <c r="B114" t="s">
+        <v>23</v>
+      </c>
+      <c r="C114" t="s">
+        <v>114</v>
+      </c>
+      <c r="D114" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" t="s">
+        <v>67</v>
+      </c>
+      <c r="B115" t="s">
+        <v>67</v>
+      </c>
+      <c r="C115" t="s">
+        <v>114</v>
+      </c>
+      <c r="D115" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" t="s">
         <v>104</v>
+      </c>
+      <c r="B116" t="s">
+        <v>104</v>
+      </c>
+      <c r="C116" t="s">
+        <v>114</v>
+      </c>
+      <c r="D116" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" t="s">
+        <v>23</v>
+      </c>
+      <c r="B117" t="s">
+        <v>23</v>
+      </c>
+      <c r="C117" t="s">
+        <v>114</v>
+      </c>
+      <c r="D117" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" t="s">
+        <v>93</v>
+      </c>
+      <c r="B118" t="s">
+        <v>93</v>
+      </c>
+      <c r="C118" t="s">
+        <v>114</v>
+      </c>
+      <c r="D118" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" t="s">
+        <v>105</v>
+      </c>
+      <c r="B119" t="s">
+        <v>105</v>
+      </c>
+      <c r="C119" t="s">
+        <v>114</v>
+      </c>
+      <c r="D119" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" t="s">
+        <v>106</v>
+      </c>
+      <c r="B120" t="s">
+        <v>106</v>
+      </c>
+      <c r="C120" t="s">
+        <v>114</v>
+      </c>
+      <c r="D120" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" t="s">
+        <v>107</v>
+      </c>
+      <c r="B121" t="s">
+        <v>107</v>
+      </c>
+      <c r="C121" t="s">
+        <v>114</v>
+      </c>
+      <c r="D121" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" t="s">
+        <v>108</v>
+      </c>
+      <c r="B122" t="s">
+        <v>108</v>
+      </c>
+      <c r="C122" t="s">
+        <v>114</v>
+      </c>
+      <c r="D122" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" t="s">
+        <v>23</v>
+      </c>
+      <c r="B123" t="s">
+        <v>23</v>
+      </c>
+      <c r="C123" t="s">
+        <v>114</v>
+      </c>
+      <c r="D123" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" t="s">
+        <v>67</v>
+      </c>
+      <c r="B124" t="s">
+        <v>67</v>
+      </c>
+      <c r="C124" t="s">
+        <v>114</v>
+      </c>
+      <c r="D124" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" t="s">
+        <v>109</v>
+      </c>
+      <c r="B125" t="s">
+        <v>109</v>
+      </c>
+      <c r="C125" t="s">
+        <v>114</v>
+      </c>
+      <c r="D125" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" t="s">
+        <v>110</v>
+      </c>
+      <c r="B126" t="s">
+        <v>110</v>
+      </c>
+      <c r="C126" t="s">
+        <v>114</v>
+      </c>
+      <c r="D126" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" t="s">
+        <v>111</v>
+      </c>
+      <c r="B127" t="s">
+        <v>111</v>
+      </c>
+      <c r="C127" t="s">
+        <v>114</v>
+      </c>
+      <c r="D127" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" t="s">
+        <v>112</v>
+      </c>
+      <c r="B128" t="s">
+        <v>112</v>
+      </c>
+      <c r="C128" t="s">
+        <v>114</v>
+      </c>
+      <c r="D128" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" t="s">
+        <v>111</v>
+      </c>
+      <c r="B129" t="s">
+        <v>111</v>
+      </c>
+      <c r="C129" t="s">
+        <v>114</v>
+      </c>
+      <c r="D129" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" t="s">
+        <v>113</v>
+      </c>
+      <c r="B130" t="s">
+        <v>113</v>
+      </c>
+      <c r="C130" t="s">
+        <v>114</v>
+      </c>
+      <c r="D130" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -4117,13 +4744,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.8100000000000001</v>
+        <v>0.74</v>
       </c>
       <c r="C4">
         <v>0.84</v>
       </c>
       <c r="D4">
-        <v>0.83</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4173,13 +4800,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>0.59</v>
+        <v>0.58</v>
       </c>
       <c r="C8">
         <v>0.77</v>
       </c>
       <c r="D8">
-        <v>0.43</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4190,10 +4817,10 @@
         <v>0.86</v>
       </c>
       <c r="C9">
-        <v>0.8</v>
+        <v>0.76</v>
       </c>
       <c r="D9">
-        <v>0.83</v>
+        <v>0.8100000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -4203,7 +4830,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4231,7 +4858,7 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -4245,7 +4872,7 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -4259,7 +4886,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -4267,10 +4894,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -4281,13 +4908,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -4295,10 +4922,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -4332,7 +4959,7 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4346,7 +4973,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -4357,7 +4984,7 @@
         <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
@@ -4374,21 +5001,21 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4402,7 +5029,7 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4416,21 +5043,21 @@
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4444,15 +5071,15 @@
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -4469,7 +5096,7 @@
         <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
@@ -4511,7 +5138,7 @@
         <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D22" t="s">
         <v>6</v>
@@ -4533,16 +5160,16 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="B24" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -4553,7 +5180,7 @@
         <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
@@ -4567,7 +5194,7 @@
         <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -4581,7 +5208,7 @@
         <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
@@ -4598,7 +5225,7 @@
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -4612,7 +5239,7 @@
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -4626,7 +5253,7 @@
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -4640,7 +5267,7 @@
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -4654,7 +5281,7 @@
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -4668,7 +5295,7 @@
         <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -4682,7 +5309,7 @@
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -4696,7 +5323,7 @@
         <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -4710,7 +5337,7 @@
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -4724,7 +5351,7 @@
         <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -4735,7 +5362,7 @@
         <v>61</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D38" t="s">
         <v>9</v>
@@ -4752,21 +5379,147 @@
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="B40" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>101</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -4798,7 +5551,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="B2">
         <v>0.86</v>
@@ -4812,7 +5565,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4826,16 +5579,16 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="B4">
-        <v>0.87</v>
+        <v>0.82</v>
       </c>
       <c r="C4">
         <v>0.9</v>
       </c>
       <c r="D4">
-        <v>0.89</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4843,13 +5596,13 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.58</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="C5">
         <v>0.88</v>
       </c>
       <c r="D5">
-        <v>0.5600000000000001</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4860,10 +5613,10 @@
         <v>0.89</v>
       </c>
       <c r="C6">
+        <v>0.79</v>
+      </c>
+      <c r="D6">
         <v>0.83</v>
-      </c>
-      <c r="D6">
-        <v>0.86</v>
       </c>
     </row>
   </sheetData>
@@ -4873,7 +5626,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4901,10 +5654,10 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4915,10 +5668,10 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4929,24 +5682,24 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4957,10 +5710,10 @@
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4971,10 +5724,10 @@
         <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4985,10 +5738,10 @@
         <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4999,10 +5752,10 @@
         <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D9" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5013,24 +5766,24 @@
         <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D10" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D11" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -5041,10 +5794,10 @@
         <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D12" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -5055,24 +5808,24 @@
         <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D13" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D14" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -5083,10 +5836,10 @@
         <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D15" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -5097,10 +5850,10 @@
         <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D16" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -5111,10 +5864,10 @@
         <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D17" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -5125,10 +5878,10 @@
         <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D18" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -5139,24 +5892,24 @@
         <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D19" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D20" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -5167,10 +5920,10 @@
         <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D21" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -5181,10 +5934,10 @@
         <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D22" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -5195,10 +5948,10 @@
         <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D23" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -5209,10 +5962,10 @@
         <v>70</v>
       </c>
       <c r="C24" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D24" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -5223,10 +5976,10 @@
         <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D25" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -5237,10 +5990,10 @@
         <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D26" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -5251,10 +6004,10 @@
         <v>77</v>
       </c>
       <c r="C27" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D27" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -5265,10 +6018,10 @@
         <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D28" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5279,10 +6032,10 @@
         <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D29" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -5293,10 +6046,10 @@
         <v>76</v>
       </c>
       <c r="C30" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D30" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5307,10 +6060,10 @@
         <v>77</v>
       </c>
       <c r="C31" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D31" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -5321,10 +6074,10 @@
         <v>79</v>
       </c>
       <c r="C32" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D32" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -5335,10 +6088,10 @@
         <v>85</v>
       </c>
       <c r="C33" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D33" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -5349,10 +6102,10 @@
         <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="D34" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -5363,24 +6116,150 @@
         <v>94</v>
       </c>
       <c r="C35" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D35" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="B36" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="C36" t="s">
+        <v>117</v>
+      </c>
+      <c r="D36" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" t="s">
+        <v>117</v>
+      </c>
+      <c r="D38" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
         <v>104</v>
       </c>
-      <c r="D36" t="s">
-        <v>101</v>
+      <c r="B41" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" t="s">
+        <v>117</v>
+      </c>
+      <c r="D45" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>